<commit_message>
add changes detail finish
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\supervisor_module\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\supervisor_module_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF99990-E706-484D-96BD-82A45274FCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CAF981-5A0C-45D0-93F4-6A2069076984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -55,24 +55,12 @@
   <si>
     <t>contrasena</t>
   </si>
-  <si>
-    <t>benito</t>
-  </si>
-  <si>
-    <t>camela</t>
-  </si>
-  <si>
-    <t>benito@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>202365benito</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,9 +69,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,18 +100,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,15 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAD9A26-B18F-4720-A080-BCFDDAD853DF}">
-  <dimension ref="A1:J2"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,32 +473,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>10256325</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{42A18433-1351-4FF3-9874-CCD1CB667423}"/>
-  </hyperlinks>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error al validar datos" error="Ingresa solo letras, sin números ni caracteres especiales" sqref="B2:B1048576" xr:uid="{8DC57E0E-775E-4078-9327-E9B8CADAB7C7}">
+      <formula1>ISTEXT(B2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error al validar los datos" error="Ingresa solo letras, sin números ni caracteres especiales" sqref="C2:C1048576" xr:uid="{BAB7F50F-2438-4890-AD3B-0AAA551231EC}">
+      <formula1>ISTEXT(C2)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error al validar los datos" error="Debe ser un número entero mayor que 0" sqref="A2:A1048576" xr:uid="{4125FA77-E5E5-4F08-881F-AB7AFF6FA5E4}">
+      <formula1>AND(ISNUMBER(A2), A2&gt;0)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error al validar los datos" error="Debe ser un número entero con 8 a 10 dígitos." sqref="D2:D1048576" xr:uid="{1216B6F0-8DC5-4967-8039-4FAFBA1B2EF5}">
+      <formula1>AND(ISNUMBER(D2), OR(LEN(D2)=8, LEN(D2)=10))</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error al validar los datos" error="Correo Electrónico (Debe tener formato válido)" sqref="E2:E1048576" xr:uid="{13748F37-0D68-4BCD-95E6-9D0C292E7BFD}">
+      <formula1>AND(ISTEXT(E2), SEARCH("@", E2)&gt;1, SEARCH(".", E2) &gt; SEARCH("@", E2)+1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error al validar los datos" error="Contraseña (Debe tener al menos 8 caracteres)" sqref="F2:F1048576" xr:uid="{D9CDC789-CA80-4E74-9F73-DA4A02EEF832}">
+      <formula1>LEN(F2)&gt;=8</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>